<commit_message>
Inicio proceso de nuevas cedulas, solo las primeras 40, se incluye la lista de todas las cedulas del ultimo script
</commit_message>
<xml_diff>
--- a/cedulas_Procesadas.xlsx
+++ b/cedulas_Procesadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ContratosSuperflex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2018FA7-017E-4EF3-B4AE-72EE2B964BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D888016-AE5D-4471-B0B2-8238D9EAFB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>VILLAVICENCIO 1</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>23/08/20225</t>
+  </si>
+  <si>
+    <t>TODAS LAS ROJAS PENDIENTES POR CERRAR SESION CON OPCION 15</t>
   </si>
 </sst>
 </file>
@@ -72,7 +75,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +100,12 @@
         <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -111,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -119,6 +128,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,15 +412,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F874"/>
+  <dimension ref="A1:F1128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A669" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A684" sqref="A684:A874"/>
+    <sheetView tabSelected="1" topLeftCell="A1075" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1086" sqref="B1086"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="24.81640625" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" customWidth="1"/>
+    <col min="2" max="2" width="58.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="17.90625" customWidth="1"/>
   </cols>
@@ -4794,7 +4807,1311 @@
         <v>1007437551</v>
       </c>
     </row>
+    <row r="876" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A876" s="1">
+        <v>45931</v>
+      </c>
+    </row>
+    <row r="877" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A877" s="3">
+        <v>30080356</v>
+      </c>
+    </row>
+    <row r="878" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A878" s="5">
+        <v>21229026</v>
+      </c>
+    </row>
+    <row r="879" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A879" s="5">
+        <v>39727147</v>
+      </c>
+    </row>
+    <row r="880" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A880" s="5">
+        <v>17329021</v>
+      </c>
+    </row>
+    <row r="881" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A881" s="5">
+        <v>39728361</v>
+      </c>
+    </row>
+    <row r="882" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A882" s="3">
+        <v>40367231</v>
+      </c>
+    </row>
+    <row r="883" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A883" s="5">
+        <v>37671025</v>
+      </c>
+    </row>
+    <row r="884" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A884" s="3">
+        <v>40188151</v>
+      </c>
+    </row>
+    <row r="885" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A885" s="5">
+        <v>40334977</v>
+      </c>
+    </row>
+    <row r="886" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A886" s="3">
+        <v>1120498000</v>
+      </c>
+    </row>
+    <row r="887" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A887" s="3">
+        <v>40403787</v>
+      </c>
+    </row>
+    <row r="888" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A888" s="3">
+        <v>1121891980</v>
+      </c>
+    </row>
+    <row r="889" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A889" s="3">
+        <v>1121864632</v>
+      </c>
+    </row>
+    <row r="890" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A890" s="3">
+        <v>40332711</v>
+      </c>
+    </row>
+    <row r="891" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A891" s="3">
+        <v>1121847839</v>
+      </c>
+    </row>
+    <row r="892" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A892" s="5">
+        <v>40413367</v>
+      </c>
+    </row>
+    <row r="893" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A893" s="3">
+        <v>39648983</v>
+      </c>
+    </row>
+    <row r="894" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A894" s="3">
+        <v>1007702703</v>
+      </c>
+    </row>
+    <row r="895" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A895" s="5">
+        <v>40218053</v>
+      </c>
+    </row>
+    <row r="896" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A896" s="3">
+        <v>1006442026</v>
+      </c>
+    </row>
+    <row r="897" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A897" s="5">
+        <v>1121892958</v>
+      </c>
+    </row>
+    <row r="898" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A898" s="3">
+        <v>1072395724</v>
+      </c>
+    </row>
+    <row r="899" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A899" s="3">
+        <v>1143252992</v>
+      </c>
+    </row>
+    <row r="900" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A900" s="3">
+        <v>35261784</v>
+      </c>
+    </row>
+    <row r="901" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A901" s="3">
+        <v>40394987</v>
+      </c>
+    </row>
+    <row r="902" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A902" s="3">
+        <v>40442006</v>
+      </c>
+    </row>
+    <row r="903" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A903" s="3">
+        <v>1001118801</v>
+      </c>
+    </row>
+    <row r="904" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A904" s="3">
+        <v>40390505</v>
+      </c>
+    </row>
+    <row r="905" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A905" s="3">
+        <v>1121955504</v>
+      </c>
+    </row>
+    <row r="906" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A906" s="3">
+        <v>1000832681</v>
+      </c>
+    </row>
+    <row r="907" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A907" s="3">
+        <v>1121849388</v>
+      </c>
+    </row>
+    <row r="908" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A908" s="3">
+        <v>1121818890</v>
+      </c>
+    </row>
+    <row r="909" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A909" s="3">
+        <v>1121954646</v>
+      </c>
+    </row>
+    <row r="910" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A910" s="5">
+        <v>21242719</v>
+      </c>
+    </row>
+    <row r="911" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A911" s="3">
+        <v>1121844971</v>
+      </c>
+    </row>
+    <row r="912" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A912" s="3">
+        <v>40215468</v>
+      </c>
+    </row>
+    <row r="913" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A913" s="3">
+        <v>1075277227</v>
+      </c>
+    </row>
+    <row r="914" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A914" s="3">
+        <v>1118291987</v>
+      </c>
+    </row>
+    <row r="915" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A915" s="3">
+        <v>1121873859</v>
+      </c>
+    </row>
+    <row r="916" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A916" s="3">
+        <v>1121821756</v>
+      </c>
+    </row>
+    <row r="917" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A917" s="3">
+        <v>1122653540</v>
+      </c>
+    </row>
+    <row r="918" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A918" s="3">
+        <v>86086391</v>
+      </c>
+    </row>
+    <row r="919" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A919" s="3">
+        <v>1006828058</v>
+      </c>
+    </row>
+    <row r="920" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A920" s="3">
+        <v>1121871447</v>
+      </c>
+    </row>
+    <row r="921" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A921" s="3">
+        <v>40218016</v>
+      </c>
+    </row>
+    <row r="922" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A922" s="3">
+        <v>1121917747</v>
+      </c>
+    </row>
+    <row r="923" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A923" s="3">
+        <v>1121827017</v>
+      </c>
+    </row>
+    <row r="924" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A924" s="3">
+        <v>1121862649</v>
+      </c>
+    </row>
+    <row r="925" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A925" s="3">
+        <v>1006798198</v>
+      </c>
+    </row>
+    <row r="926" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A926" s="5">
+        <v>1121852594</v>
+      </c>
+    </row>
+    <row r="927" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A927" s="3">
+        <v>1121946818</v>
+      </c>
+    </row>
+    <row r="928" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A928" s="5">
+        <v>1125552959</v>
+      </c>
+    </row>
+    <row r="929" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A929" s="3">
+        <v>40331222</v>
+      </c>
+    </row>
+    <row r="930" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A930" s="5">
+        <v>1056782595</v>
+      </c>
+    </row>
+    <row r="931" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A931" s="3">
+        <v>1006772734</v>
+      </c>
+    </row>
+    <row r="932" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A932" s="3">
+        <v>1121893657</v>
+      </c>
+    </row>
+    <row r="933" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A933" s="3">
+        <v>1121849200</v>
+      </c>
+    </row>
+    <row r="934" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A934" s="3">
+        <v>1014184746</v>
+      </c>
+    </row>
+    <row r="935" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A935" s="5">
+        <v>1023035549</v>
+      </c>
+    </row>
+    <row r="936" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A936" s="5">
+        <v>1007413869</v>
+      </c>
+    </row>
+    <row r="937" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A937" s="3">
+        <v>1006828141</v>
+      </c>
+    </row>
+    <row r="938" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A938" s="5">
+        <v>1122138078</v>
+      </c>
+    </row>
+    <row r="939" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A939" s="3">
+        <v>1121896390</v>
+      </c>
+    </row>
+    <row r="940" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A940" s="5">
+        <v>40401474</v>
+      </c>
+    </row>
+    <row r="941" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A941" s="3">
+        <v>1121824236</v>
+      </c>
+    </row>
+    <row r="942" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A942" s="3">
+        <v>1123561577</v>
+      </c>
+    </row>
+    <row r="943" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A943" s="3">
+        <v>40325807</v>
+      </c>
+    </row>
+    <row r="944" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A944" s="3">
+        <v>40441092</v>
+      </c>
+    </row>
+    <row r="945" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A945" s="5">
+        <v>38290869</v>
+      </c>
+    </row>
+    <row r="946" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A946" s="3">
+        <v>1123801589</v>
+      </c>
+    </row>
+    <row r="947" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A947" s="3">
+        <v>1127391633</v>
+      </c>
+    </row>
+    <row r="948" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A948" s="5">
+        <v>40386471</v>
+      </c>
+    </row>
+    <row r="949" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A949" s="3">
+        <v>1030623737</v>
+      </c>
+    </row>
+    <row r="950" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A950" s="5">
+        <v>40388244</v>
+      </c>
+    </row>
+    <row r="951" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A951" s="3">
+        <v>52977026</v>
+      </c>
+    </row>
+    <row r="952" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A952" s="3">
+        <v>52862750</v>
+      </c>
+    </row>
+    <row r="953" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A953" s="3">
+        <v>1007741689</v>
+      </c>
+    </row>
+    <row r="954" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A954" s="3">
+        <v>40189602</v>
+      </c>
+    </row>
+    <row r="955" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A955" s="3">
+        <v>1234790567</v>
+      </c>
+    </row>
+    <row r="956" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A956" s="3">
+        <v>1006335084</v>
+      </c>
+    </row>
+    <row r="957" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A957" s="3">
+        <v>1234789507</v>
+      </c>
+    </row>
+    <row r="958" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A958" s="3">
+        <v>1033748818</v>
+      </c>
+    </row>
+    <row r="959" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A959" s="5">
+        <v>1121946821</v>
+      </c>
+    </row>
+    <row r="960" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A960" s="3">
+        <v>1121915532</v>
+      </c>
+    </row>
+    <row r="961" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A961" s="3">
+        <v>1120378354</v>
+      </c>
+    </row>
+    <row r="962" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A962" s="5">
+        <v>1007816099</v>
+      </c>
+    </row>
+    <row r="963" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A963" s="3">
+        <v>1005566462</v>
+      </c>
+    </row>
+    <row r="964" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A964" s="3">
+        <v>1005294945</v>
+      </c>
+    </row>
+    <row r="965" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A965" s="3">
+        <v>1122655308</v>
+      </c>
+    </row>
+    <row r="966" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A966" s="3">
+        <v>1006775023</v>
+      </c>
+    </row>
+    <row r="967" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A967" s="5">
+        <v>1006797846</v>
+      </c>
+    </row>
+    <row r="968" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A968" s="3">
+        <v>1003583504</v>
+      </c>
+    </row>
+    <row r="969" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A969" s="3">
+        <v>1121146010</v>
+      </c>
+    </row>
+    <row r="970" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A970" s="3">
+        <v>1122653301</v>
+      </c>
+    </row>
+    <row r="971" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A971" s="3">
+        <v>40186992</v>
+      </c>
+    </row>
+    <row r="972" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A972" s="3">
+        <v>1010123626</v>
+      </c>
+    </row>
+    <row r="973" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A973" s="3">
+        <v>1234789441</v>
+      </c>
+    </row>
+    <row r="974" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A974" s="3">
+        <v>1123431666</v>
+      </c>
+    </row>
+    <row r="975" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A975" s="3">
+        <v>1006859731</v>
+      </c>
+    </row>
+    <row r="976" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A976" s="3">
+        <v>1120385112</v>
+      </c>
+    </row>
+    <row r="977" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A977" s="3">
+        <v>1121921356</v>
+      </c>
+    </row>
+    <row r="978" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A978" s="5">
+        <v>1006774144</v>
+      </c>
+    </row>
+    <row r="979" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A979" s="3">
+        <v>1123140904</v>
+      </c>
+    </row>
+    <row r="980" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A980" s="3">
+        <v>1010031875</v>
+      </c>
+    </row>
+    <row r="981" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A981" s="3">
+        <v>46376887</v>
+      </c>
+    </row>
+    <row r="982" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A982" s="3">
+        <v>1006820624</v>
+      </c>
+    </row>
+    <row r="983" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A983" s="3">
+        <v>1121833506</v>
+      </c>
+    </row>
+    <row r="984" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A984" s="3">
+        <v>1121888058</v>
+      </c>
+    </row>
+    <row r="985" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A985" s="3">
+        <v>1122919487</v>
+      </c>
+    </row>
+    <row r="986" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A986" s="3">
+        <v>1193221023</v>
+      </c>
+    </row>
+    <row r="987" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A987" s="5">
+        <v>1121872788</v>
+      </c>
+    </row>
+    <row r="988" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A988" s="3">
+        <v>1069735886</v>
+      </c>
+    </row>
+    <row r="989" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A989" s="3">
+        <v>1007437551</v>
+      </c>
+    </row>
+    <row r="990" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A990" s="3">
+        <v>1121931106</v>
+      </c>
+    </row>
+    <row r="991" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A991" s="3">
+        <v>1014243158</v>
+      </c>
+    </row>
+    <row r="992" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A992" s="3">
+        <v>1121944349</v>
+      </c>
+    </row>
+    <row r="993" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A993" s="3">
+        <v>1000580172</v>
+      </c>
+    </row>
+    <row r="994" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A994" s="3">
+        <v>1085280827</v>
+      </c>
+    </row>
+    <row r="995" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A995" s="3">
+        <v>1014292653</v>
+      </c>
+    </row>
+    <row r="996" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A996" s="3">
+        <v>52710556</v>
+      </c>
+    </row>
+    <row r="997" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A997" s="3">
+        <v>1121822749</v>
+      </c>
+    </row>
+    <row r="998" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A998" s="3">
+        <v>1001174715</v>
+      </c>
+    </row>
+    <row r="999" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A999" s="3">
+        <v>1123430278</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1000" s="3">
+        <v>1022408192</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1001" s="3">
+        <v>1121836926</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1002" s="3">
+        <v>40333112</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1003" s="3">
+        <v>1127382143</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1004" s="3">
+        <v>1002577155</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1005" s="5">
+        <v>24100971</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1006" s="3">
+        <v>1002085841</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1007" s="3">
+        <v>1121935079</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1008" s="3">
+        <v>1006827679</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1009" s="3">
+        <v>1006736555</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1010" s="3">
+        <v>1029982510</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1011" s="3">
+        <v>1001885026</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1012" s="3">
+        <v>1121960484</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1013" s="3">
+        <v>1007702953</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1014" s="3">
+        <v>1006722113</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1015" s="5">
+        <v>1029981260</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1016" s="3">
+        <v>1007730620</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1017" s="3">
+        <v>1007318395</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1018" s="3">
+        <v>1121923083</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1019" s="3">
+        <v>1014306063</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1020">
+        <v>1097990010</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1021" s="3">
+        <v>1121919401</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1022" s="3">
+        <v>1022341095</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1023" s="3">
+        <v>1233490733</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1024" s="3">
+        <v>1123803651</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1025" s="3">
+        <v>39570143</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1026" s="5">
+        <v>1121849836</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1027" s="3">
+        <v>1029982301</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1028" s="3">
+        <v>52483077</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1029" s="3">
+        <v>1121146397</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1030" s="3">
+        <v>1006658626</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1031" s="3">
+        <v>40439256</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1032" s="5">
+        <v>52501176</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1033" s="3">
+        <v>1121834547</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1034" s="3">
+        <v>1122507401</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1035" s="3">
+        <v>1121940276</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1036" s="3">
+        <v>1122507035</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1037" s="3">
+        <v>1013674750</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1038" s="3">
+        <v>1122511768</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1039" s="3">
+        <v>1122918696</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1040" s="3">
+        <v>1120926035</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1041" s="5">
+        <v>1121830619</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1042" s="3">
+        <v>77777780</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1043" s="3">
+        <v>1022960497</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1044" s="3">
+        <v>1113692397</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1045" s="3">
+        <v>1036840503</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1046" s="3">
+        <v>1006695715</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1047" s="3">
+        <v>63471947</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1048" s="3">
+        <v>1121965996</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1049" s="3">
+        <v>1006692119</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1050" s="3">
+        <v>1121931253</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1051" s="3">
+        <v>40333161</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1052" s="3">
+        <v>1120870248</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1053" s="3">
+        <v>1120871550</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1054" s="3">
+        <v>1123860010</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1055" s="5">
+        <v>1077976735</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1056" s="3">
+        <v>1234789628</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1057" s="3">
+        <v>1065644681</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1058" s="3">
+        <v>1006819843</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1059" s="5">
+        <v>1005159244</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1060" s="5">
+        <v>1006794572</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1061" s="5">
+        <v>1006824446</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1062" s="3">
+        <v>1193092480</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1063" s="5">
+        <v>1121915979</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1064" s="3">
+        <v>1122647759</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1065" s="3">
+        <v>1121874758</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1066" s="3">
+        <v>1005848328</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1067" s="3">
+        <v>1121416122</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1068" s="3">
+        <v>1007584794</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1069" s="3">
+        <v>1121927207</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1070" s="3">
+        <v>1122918521</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1071" s="3">
+        <v>1003565669</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1072" s="3">
+        <v>1106775925</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1073" s="3">
+        <v>1121966736</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1074" s="3">
+        <v>1121931564</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1075" s="3">
+        <v>1121817727</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1076" s="5">
+        <v>1022999589</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1077" s="5">
+        <v>1006656639</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1078" s="5">
+        <v>1096196072</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1079" s="3">
+        <v>1122511568</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1080" s="3">
+        <v>1118532809</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1081" s="3">
+        <v>1006796310</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1082" s="3">
+        <v>53062799</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1083" s="3">
+        <v>1106888062</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1084" s="3">
+        <v>1121844532</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1085" s="5">
+        <v>1034660761</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1086" s="3">
+        <v>1005848329</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1087" s="3">
+        <v>1121817958</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1089" s="1">
+        <v>45932</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1090" s="5">
+        <v>21229026</v>
+      </c>
+      <c r="B1090" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1091" s="5">
+        <v>39727147</v>
+      </c>
+      <c r="B1091" s="7"/>
+    </row>
+    <row r="1092" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1092" s="5">
+        <v>17329021</v>
+      </c>
+      <c r="B1092" s="7"/>
+    </row>
+    <row r="1093" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1093" s="5">
+        <v>39728361</v>
+      </c>
+      <c r="B1093" s="7"/>
+    </row>
+    <row r="1094" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1094" s="5">
+        <v>37671025</v>
+      </c>
+      <c r="B1094" s="7"/>
+    </row>
+    <row r="1095" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1095" s="5">
+        <v>40334977</v>
+      </c>
+      <c r="B1095" s="7"/>
+    </row>
+    <row r="1096" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1096" s="5">
+        <v>40413367</v>
+      </c>
+      <c r="B1096" s="7"/>
+    </row>
+    <row r="1097" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1097" s="3">
+        <v>40218053</v>
+      </c>
+      <c r="B1097" s="7"/>
+    </row>
+    <row r="1098" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1098" s="5">
+        <v>1121892958</v>
+      </c>
+      <c r="B1098" s="7"/>
+    </row>
+    <row r="1099" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1099" s="5">
+        <v>21242719</v>
+      </c>
+      <c r="B1099" s="7"/>
+    </row>
+    <row r="1100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1100" s="3">
+        <v>1121852594</v>
+      </c>
+      <c r="B1100" s="7"/>
+    </row>
+    <row r="1101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1101" s="5">
+        <v>1125552959</v>
+      </c>
+      <c r="B1101" s="7"/>
+    </row>
+    <row r="1102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1102" s="5">
+        <v>1056782595</v>
+      </c>
+      <c r="B1102" s="7"/>
+    </row>
+    <row r="1103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1103" s="5">
+        <v>1023035549</v>
+      </c>
+      <c r="B1103" s="7"/>
+    </row>
+    <row r="1104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1104" s="5">
+        <v>1007413869</v>
+      </c>
+      <c r="B1104" s="7"/>
+    </row>
+    <row r="1105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1105" s="5">
+        <v>1122138078</v>
+      </c>
+      <c r="B1105" s="7"/>
+    </row>
+    <row r="1106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1106" s="5">
+        <v>40401474</v>
+      </c>
+      <c r="B1106" s="7"/>
+    </row>
+    <row r="1107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1107" s="5">
+        <v>38290869</v>
+      </c>
+      <c r="B1107" s="7"/>
+    </row>
+    <row r="1108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1108" s="5">
+        <v>40386471</v>
+      </c>
+      <c r="B1108" s="7"/>
+    </row>
+    <row r="1109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1109" s="3">
+        <v>40388244</v>
+      </c>
+      <c r="B1109" s="7"/>
+    </row>
+    <row r="1110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1110" s="5">
+        <v>1121946821</v>
+      </c>
+      <c r="B1110" s="7"/>
+    </row>
+    <row r="1111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1111" s="5">
+        <v>1007816099</v>
+      </c>
+      <c r="B1111" s="7"/>
+    </row>
+    <row r="1112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1112" s="5">
+        <v>1006797846</v>
+      </c>
+      <c r="B1112" s="7"/>
+    </row>
+    <row r="1113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1113" s="5">
+        <v>1006774144</v>
+      </c>
+      <c r="B1113" s="7"/>
+    </row>
+    <row r="1114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1114" s="5">
+        <v>1121872788</v>
+      </c>
+      <c r="B1114" s="7"/>
+    </row>
+    <row r="1115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1115" s="5">
+        <v>24100971</v>
+      </c>
+      <c r="B1115" s="7"/>
+    </row>
+    <row r="1116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1116" s="5">
+        <v>1029981260</v>
+      </c>
+      <c r="B1116" s="7"/>
+    </row>
+    <row r="1117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1117" s="3">
+        <v>1097990010</v>
+      </c>
+      <c r="B1117" s="7"/>
+    </row>
+    <row r="1118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1118" s="3">
+        <v>52501176</v>
+      </c>
+      <c r="B1118" s="7"/>
+    </row>
+    <row r="1119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1119" s="5">
+        <v>1121830619</v>
+      </c>
+      <c r="B1119" s="7"/>
+    </row>
+    <row r="1120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1120" s="5">
+        <v>1077976735</v>
+      </c>
+      <c r="B1120" s="7"/>
+    </row>
+    <row r="1121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1121" s="5">
+        <v>1005159244</v>
+      </c>
+      <c r="B1121" s="7"/>
+    </row>
+    <row r="1122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1122" s="5">
+        <v>1006794572</v>
+      </c>
+      <c r="B1122" s="7"/>
+    </row>
+    <row r="1123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1123" s="5">
+        <v>1006824446</v>
+      </c>
+      <c r="B1123" s="7"/>
+    </row>
+    <row r="1124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1124" s="3">
+        <v>1121915979</v>
+      </c>
+      <c r="B1124" s="7"/>
+    </row>
+    <row r="1125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1125" s="5">
+        <v>1022999589</v>
+      </c>
+      <c r="B1125" s="7"/>
+    </row>
+    <row r="1126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1126" s="5">
+        <v>1006656639</v>
+      </c>
+      <c r="B1126" s="7"/>
+    </row>
+    <row r="1127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1127" s="5">
+        <v>1096196072</v>
+      </c>
+      <c r="B1127" s="7"/>
+    </row>
+    <row r="1128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1128" s="5">
+        <v>1034660761</v>
+      </c>
+      <c r="B1128" s="7"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1090:B1128"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="2321" orientation="portrait" horizontalDpi="160" verticalDpi="144" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
creando funcionalidad de cerrar sesion
</commit_message>
<xml_diff>
--- a/cedulas_Procesadas.xlsx
+++ b/cedulas_Procesadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ContratosSuperflex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D888016-AE5D-4471-B0B2-8238D9EAFB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E163864B-667F-4DF7-8EB3-08BDD9C8B3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>VILLAVICENCIO 1</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>TODAS LAS ROJAS PENDIENTES POR CERRAR SESION CON OPCION 15</t>
+  </si>
+  <si>
+    <t>2:25pm</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1128"/>
+  <dimension ref="A1:F1170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1075" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1086" sqref="B1086"/>
+    <sheetView tabSelected="1" topLeftCell="A1123" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1134" sqref="B1134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6108,6 +6111,214 @@
       </c>
       <c r="B1128" s="7"/>
     </row>
+    <row r="1130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1130" s="1">
+        <v>45932</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1131" s="5">
+        <v>21205258</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1132" s="3">
+        <v>31006459</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1133" s="3">
+        <v>21177007</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1134" s="5">
+        <v>17360686</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1135" s="5">
+        <v>51642333</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1136" s="3">
+        <v>21199606</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1137" s="5">
+        <v>3292415</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1138" s="5">
+        <v>11373533</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1139" s="5">
+        <v>30030456</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1140" s="5">
+        <v>70052315</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1141" s="5">
+        <v>3282146</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1142" s="5">
+        <v>3045925</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1143" s="5">
+        <v>21173140</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1144" s="5">
+        <v>21234532</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1145" s="5">
+        <v>6671921</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1146" s="3">
+        <v>86010008</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1147" s="5">
+        <v>4561950</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1148" s="3">
+        <v>1119886285</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1149" s="5">
+        <v>40422362</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1150" s="5">
+        <v>40447756</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1151" s="3">
+        <v>1122649188</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1152" s="3">
+        <v>21182125</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1153" s="3">
+        <v>30001167</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1154" s="3">
+        <v>1122129288</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1155" s="3">
+        <v>1122646151</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1156" s="3">
+        <v>1122652108</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1157" s="3">
+        <v>40315281</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1158" s="5">
+        <v>19337954</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1159" s="5">
+        <v>30055021</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1160" s="3">
+        <v>40362749</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1161" s="5">
+        <v>40446257</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1162" s="5">
+        <v>40434896</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1163" s="3">
+        <v>1123058626</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1164" s="3">
+        <v>1122134224</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1165" s="5">
+        <v>1123860656</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1166" s="5">
+        <v>30055352</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1167" s="5">
+        <v>40362705</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1168" s="3">
+        <v>40449564</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1169" s="3">
+        <v>23629227</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1170" s="3">
+        <v>1120499341</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1090:B1128"/>

</xml_diff>

<commit_message>
Cedulas pendientes por cerrar sesion
</commit_message>
<xml_diff>
--- a/cedulas_Procesadas.xlsx
+++ b/cedulas_Procesadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ContratosSuperflex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E163864B-667F-4DF7-8EB3-08BDD9C8B3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54956A07-0C8F-45D6-A6BD-5737F73DB889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>VILLAVICENCIO 1</t>
   </si>
@@ -50,12 +50,15 @@
   <si>
     <t>2:25pm</t>
   </si>
+  <si>
+    <t>3/10/2025 1:38PM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +79,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -123,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -131,6 +140,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -415,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1170"/>
+  <dimension ref="A1:F1484"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1123" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1134" sqref="B1134"/>
+    <sheetView tabSelected="1" topLeftCell="A1427" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K1444" sqref="K1444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5879,7 +5890,7 @@
       <c r="A1090" s="5">
         <v>21229026</v>
       </c>
-      <c r="B1090" s="7" t="s">
+      <c r="B1090" s="9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5887,229 +5898,229 @@
       <c r="A1091" s="5">
         <v>39727147</v>
       </c>
-      <c r="B1091" s="7"/>
+      <c r="B1091" s="9"/>
     </row>
     <row r="1092" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1092" s="5">
         <v>17329021</v>
       </c>
-      <c r="B1092" s="7"/>
+      <c r="B1092" s="9"/>
     </row>
     <row r="1093" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1093" s="5">
         <v>39728361</v>
       </c>
-      <c r="B1093" s="7"/>
+      <c r="B1093" s="9"/>
     </row>
     <row r="1094" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1094" s="5">
         <v>37671025</v>
       </c>
-      <c r="B1094" s="7"/>
+      <c r="B1094" s="9"/>
     </row>
     <row r="1095" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1095" s="5">
         <v>40334977</v>
       </c>
-      <c r="B1095" s="7"/>
+      <c r="B1095" s="9"/>
     </row>
     <row r="1096" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1096" s="5">
         <v>40413367</v>
       </c>
-      <c r="B1096" s="7"/>
+      <c r="B1096" s="9"/>
     </row>
     <row r="1097" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1097" s="3">
         <v>40218053</v>
       </c>
-      <c r="B1097" s="7"/>
+      <c r="B1097" s="9"/>
     </row>
     <row r="1098" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1098" s="5">
         <v>1121892958</v>
       </c>
-      <c r="B1098" s="7"/>
+      <c r="B1098" s="9"/>
     </row>
     <row r="1099" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1099" s="5">
         <v>21242719</v>
       </c>
-      <c r="B1099" s="7"/>
+      <c r="B1099" s="9"/>
     </row>
     <row r="1100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1100" s="3">
         <v>1121852594</v>
       </c>
-      <c r="B1100" s="7"/>
+      <c r="B1100" s="9"/>
     </row>
     <row r="1101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1101" s="5">
         <v>1125552959</v>
       </c>
-      <c r="B1101" s="7"/>
+      <c r="B1101" s="9"/>
     </row>
     <row r="1102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1102" s="5">
         <v>1056782595</v>
       </c>
-      <c r="B1102" s="7"/>
+      <c r="B1102" s="9"/>
     </row>
     <row r="1103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1103" s="5">
         <v>1023035549</v>
       </c>
-      <c r="B1103" s="7"/>
+      <c r="B1103" s="9"/>
     </row>
     <row r="1104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1104" s="5">
         <v>1007413869</v>
       </c>
-      <c r="B1104" s="7"/>
+      <c r="B1104" s="9"/>
     </row>
     <row r="1105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1105" s="5">
         <v>1122138078</v>
       </c>
-      <c r="B1105" s="7"/>
+      <c r="B1105" s="9"/>
     </row>
     <row r="1106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1106" s="5">
         <v>40401474</v>
       </c>
-      <c r="B1106" s="7"/>
+      <c r="B1106" s="9"/>
     </row>
     <row r="1107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1107" s="5">
         <v>38290869</v>
       </c>
-      <c r="B1107" s="7"/>
+      <c r="B1107" s="9"/>
     </row>
     <row r="1108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1108" s="5">
         <v>40386471</v>
       </c>
-      <c r="B1108" s="7"/>
+      <c r="B1108" s="9"/>
     </row>
     <row r="1109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1109" s="3">
         <v>40388244</v>
       </c>
-      <c r="B1109" s="7"/>
+      <c r="B1109" s="9"/>
     </row>
     <row r="1110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1110" s="5">
         <v>1121946821</v>
       </c>
-      <c r="B1110" s="7"/>
+      <c r="B1110" s="9"/>
     </row>
     <row r="1111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1111" s="5">
         <v>1007816099</v>
       </c>
-      <c r="B1111" s="7"/>
+      <c r="B1111" s="9"/>
     </row>
     <row r="1112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1112" s="5">
         <v>1006797846</v>
       </c>
-      <c r="B1112" s="7"/>
+      <c r="B1112" s="9"/>
     </row>
     <row r="1113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1113" s="5">
         <v>1006774144</v>
       </c>
-      <c r="B1113" s="7"/>
+      <c r="B1113" s="9"/>
     </row>
     <row r="1114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1114" s="5">
         <v>1121872788</v>
       </c>
-      <c r="B1114" s="7"/>
+      <c r="B1114" s="9"/>
     </row>
     <row r="1115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1115" s="5">
         <v>24100971</v>
       </c>
-      <c r="B1115" s="7"/>
+      <c r="B1115" s="9"/>
     </row>
     <row r="1116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1116" s="5">
         <v>1029981260</v>
       </c>
-      <c r="B1116" s="7"/>
+      <c r="B1116" s="9"/>
     </row>
     <row r="1117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1117" s="3">
         <v>1097990010</v>
       </c>
-      <c r="B1117" s="7"/>
+      <c r="B1117" s="9"/>
     </row>
     <row r="1118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1118" s="3">
         <v>52501176</v>
       </c>
-      <c r="B1118" s="7"/>
+      <c r="B1118" s="9"/>
     </row>
     <row r="1119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1119" s="5">
         <v>1121830619</v>
       </c>
-      <c r="B1119" s="7"/>
+      <c r="B1119" s="9"/>
     </row>
     <row r="1120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1120" s="5">
         <v>1077976735</v>
       </c>
-      <c r="B1120" s="7"/>
+      <c r="B1120" s="9"/>
     </row>
     <row r="1121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1121" s="5">
         <v>1005159244</v>
       </c>
-      <c r="B1121" s="7"/>
+      <c r="B1121" s="9"/>
     </row>
     <row r="1122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1122" s="5">
         <v>1006794572</v>
       </c>
-      <c r="B1122" s="7"/>
+      <c r="B1122" s="9"/>
     </row>
     <row r="1123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1123" s="5">
         <v>1006824446</v>
       </c>
-      <c r="B1123" s="7"/>
+      <c r="B1123" s="9"/>
     </row>
     <row r="1124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1124" s="3">
         <v>1121915979</v>
       </c>
-      <c r="B1124" s="7"/>
+      <c r="B1124" s="9"/>
     </row>
     <row r="1125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1125" s="5">
         <v>1022999589</v>
       </c>
-      <c r="B1125" s="7"/>
+      <c r="B1125" s="9"/>
     </row>
     <row r="1126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1126" s="5">
         <v>1006656639</v>
       </c>
-      <c r="B1126" s="7"/>
+      <c r="B1126" s="9"/>
     </row>
     <row r="1127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1127" s="5">
         <v>1096196072</v>
       </c>
-      <c r="B1127" s="7"/>
+      <c r="B1127" s="9"/>
     </row>
     <row r="1128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1128" s="5">
         <v>1034660761</v>
       </c>
-      <c r="B1128" s="7"/>
+      <c r="B1128" s="9"/>
     </row>
     <row r="1130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1130" s="1">
@@ -6317,6 +6328,1571 @@
     <row r="1170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1170" s="3">
         <v>1120499341</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1172" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1173" s="7">
+        <v>21176766</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1174" s="7">
+        <v>42986981</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1175" s="7">
+        <v>40415945</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1176" s="7">
+        <v>40448500</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1177" s="7">
+        <v>40405194</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1178" s="8">
+        <v>59671136</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1179" s="7">
+        <v>1024483160</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1180" s="8">
+        <v>21177991</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1181" s="7">
+        <v>40447815</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1182" s="8">
+        <v>14993451</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1183" s="8">
+        <v>40361978</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1184" s="7">
+        <v>86014300</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1185" s="7">
+        <v>1123084793</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1186" s="8">
+        <v>7818547</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1187" s="7">
+        <v>40413124</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1188" s="8">
+        <v>40412991</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1189" s="7">
+        <v>40215630</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1190" s="8">
+        <v>86040029</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1191" s="7">
+        <v>40447846</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1192" s="7">
+        <v>30347361</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1193" s="3">
+        <v>40429641</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1194" s="3">
+        <v>1120380003</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1195" s="5">
+        <v>40265797</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1196" s="3">
+        <v>1122132502</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1197" s="3">
+        <v>1120356609</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1198" s="3">
+        <v>31939677</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1199" s="3">
+        <v>40405846</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1200" s="3">
+        <v>1121820330</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1201" s="5">
+        <v>37559806</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1202" s="3">
+        <v>40396291</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1203" s="3">
+        <v>85449427</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1204" s="5">
+        <v>79849312</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1205" s="3">
+        <v>53093424</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1206" s="3">
+        <v>40450735</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1207" s="3">
+        <v>40266836</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1208" s="3">
+        <v>1121844576</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1209" s="3">
+        <v>31008060</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1210" s="3">
+        <v>39616373</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1211">
+        <v>1033774813</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1212" s="3">
+        <v>40432224</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1213" s="3">
+        <v>1119889226</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1214" s="3">
+        <v>1010193197</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1215" s="3">
+        <v>40422425</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1216" s="3">
+        <v>1122126675</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1217" s="3">
+        <v>52752142</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1218" s="3">
+        <v>1120353500</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1219" s="3">
+        <v>52469010</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1220" s="3">
+        <v>1122649705</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1221" s="3">
+        <v>21181515</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1222" s="5">
+        <v>1121148787</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1223" s="3">
+        <v>1006700030</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1224" s="3">
+        <v>1123530955</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1225" s="3">
+        <v>60264481</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1226" s="3">
+        <v>1073695360</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1227" s="3">
+        <v>1006449658</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1228" s="3">
+        <v>1016041709</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1229" s="3">
+        <v>1122137332</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1230" s="3">
+        <v>1122135332</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1231" s="5">
+        <v>53154537</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1232" s="3">
+        <v>1121146888</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1233" s="3">
+        <v>40185360</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1234" s="3">
+        <v>1121885145</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1235" s="3">
+        <v>40306120</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1236" s="5">
+        <v>40431599</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1237" s="5">
+        <v>30002107</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1238" s="3">
+        <v>1006689956</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1239" s="3">
+        <v>21202600</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1240">
+        <v>1121906197</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1241" s="3">
+        <v>1120356582</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1242" s="3">
+        <v>52881968</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1243" s="5">
+        <v>1000807612</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1244" s="3">
+        <v>39801680</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1245" s="3">
+        <v>1122145025</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1246" s="3">
+        <v>1121822628</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1247" s="3">
+        <v>1124217818</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1248" s="3">
+        <v>30981833</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1249" s="3">
+        <v>1126905997</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1250" s="3">
+        <v>40278351</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1251" s="5">
+        <v>31006869</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1252" s="3">
+        <v>21203424</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1253" s="3">
+        <v>1122136923</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1254" s="3">
+        <v>1124190794</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1255" s="3">
+        <v>1124243490</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1256" s="3">
+        <v>40400278</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1257" s="5">
+        <v>1124190027</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1258" s="5">
+        <v>40306131</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1259" s="3">
+        <v>1124218504</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1260" s="3">
+        <v>1124216166</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1261" s="5">
+        <v>40422019</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1262" s="5">
+        <v>1006697169</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1263" s="3">
+        <v>1122140761</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1264" s="3">
+        <v>1012425696</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1265" s="3">
+        <v>21202920</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1266" s="3">
+        <v>35255057</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1267" s="3">
+        <v>1120504924</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1268" s="3">
+        <v>1122140064</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1269" s="3">
+        <v>1127385585</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1270" s="3">
+        <v>1120384826</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1271" s="3">
+        <v>1123058967</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1272" s="3">
+        <v>40187549</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1273" s="3">
+        <v>1123115654</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1274" s="3">
+        <v>1120384377</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1275" s="3">
+        <v>40362271</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1276" s="3">
+        <v>26593620</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1277" s="5">
+        <v>1124216732</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1278" s="3">
+        <v>1120498573</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1279" s="3">
+        <v>40316428</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1280" s="3">
+        <v>1022938760</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1281" s="3">
+        <v>1074131461</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1282" s="3">
+        <v>1085343145</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1283" s="3">
+        <v>1122124846</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1284" s="3">
+        <v>1122124916</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1285" s="3">
+        <v>1122144685</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1286" s="3">
+        <v>21183385</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1287" s="3">
+        <v>1121909358</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1288" s="3">
+        <v>1122651037</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1289" s="3">
+        <v>1006779225</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1290" s="3">
+        <v>53016403</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1291" s="3">
+        <v>1120376987</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1292" s="3">
+        <v>1120387091</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1293" s="3">
+        <v>40447469</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1294" s="5">
+        <v>1120355361</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1295" s="3">
+        <v>1121931227</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1296" s="5">
+        <v>30081386</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1297" s="3">
+        <v>1122127781</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1298" s="3">
+        <v>40434094</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1299" s="3">
+        <v>40775505</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1300" s="5">
+        <v>1122138895</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1301" s="3">
+        <v>51907408</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1302" s="3">
+        <v>1123566252</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1303" s="3">
+        <v>1123566613</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1304" s="5">
+        <v>21940107</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1305" s="3">
+        <v>30030986</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1306" s="3">
+        <v>66865834</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1307" s="3">
+        <v>40447278</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1308" s="3">
+        <v>1070331092</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1309" s="3">
+        <v>1121824758</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1310" s="3">
+        <v>96195073</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1311" s="3">
+        <v>1122646913</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1312" s="3">
+        <v>1122144983</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1313" s="5">
+        <v>40187078</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1314" s="3">
+        <v>40447086</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1315" s="3">
+        <v>1124828578</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1316" s="3">
+        <v>40430721</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1317" s="3">
+        <v>40434032</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1318" s="3">
+        <v>1120506939</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1319" s="5">
+        <v>40433512</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1320" s="5">
+        <v>18598661</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1321" s="3">
+        <v>30080869</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1322" s="3">
+        <v>52116345</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1323" s="5">
+        <v>86009284</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1324" s="3">
+        <v>1119888577</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1325" s="3">
+        <v>1006904343</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1326" s="3">
+        <v>1120474468</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1327" s="3">
+        <v>1006693742</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1328" s="3">
+        <v>1120387777</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1329" s="3">
+        <v>65795239</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1330" s="3">
+        <v>1005293697</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1331" s="5">
+        <v>31006780</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1332" s="3">
+        <v>40415550</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1333" s="3">
+        <v>1122119431</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1334" s="3">
+        <v>40447519</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1335" s="5">
+        <v>28845786</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1336" s="5">
+        <v>1071304162</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1337" s="3">
+        <v>1122652696</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1338" s="3">
+        <v>1122126119</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1339" s="3">
+        <v>1122627123</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1340" s="3">
+        <v>1120373174</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1341" s="3">
+        <v>36173037</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1342" s="3">
+        <v>1023861468</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1343" s="3">
+        <v>1118535887</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1344" s="3">
+        <v>52552056</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1345" s="3">
+        <v>1123862467</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1346" s="3">
+        <v>1121903136</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1347" s="5">
+        <v>1120373472</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1348" s="3">
+        <v>1006737197</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1349" s="5">
+        <v>14952515</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1350" s="3">
+        <v>40442969</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1351" s="3">
+        <v>28907825</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1352" s="5">
+        <v>1104184087</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1353" s="5">
+        <v>1098436557</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1354" s="3">
+        <v>1120506274</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1355" s="3">
+        <v>1006877419</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1356" s="3">
+        <v>1006867028</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1357" s="5">
+        <v>21182488</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1358" s="3">
+        <v>1121923324</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1359" s="3">
+        <v>1002681230</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1360" s="3">
+        <v>1002733121</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1361" s="3">
+        <v>1121846021</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1362" s="3">
+        <v>1006903629</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1363" s="3">
+        <v>1006691122</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1364" s="5">
+        <v>1076200860</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1365" s="3">
+        <v>40393137</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1366" s="3">
+        <v>40421967</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1367" s="3">
+        <v>1006774918</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1368" s="3">
+        <v>1121823059</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1369" s="3">
+        <v>1122118438</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1370" s="3">
+        <v>1122506145</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1371" s="3">
+        <v>1006690715</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1372" s="5">
+        <v>1118562246</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1373" s="5">
+        <v>1012413227</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1374" s="5">
+        <v>1005181518</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1375" s="3">
+        <v>1120387240</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1376" s="3">
+        <v>1193581832</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1377" s="3">
+        <v>1193128654</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1378" s="3">
+        <v>31031916</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1379" s="3">
+        <v>1024516175</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1380" s="3">
+        <v>1006737670</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1381" s="3">
+        <v>1006661215</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1382" s="3">
+        <v>1122137585</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1383" s="3">
+        <v>1120378198</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1384" s="5">
+        <v>1119887995</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1385" s="5">
+        <v>1120369362</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1386" s="3">
+        <v>1006717092</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1387" s="3">
+        <v>1006729382</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1388" s="5">
+        <v>1006777681</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1389" s="3">
+        <v>40316571</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1390" s="5">
+        <v>80266280</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1391" s="3">
+        <v>1101687452</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1392" s="3">
+        <v>1006717478</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1393" s="5">
+        <v>1120362791</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1394" s="3">
+        <v>40434945</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1395" s="5">
+        <v>1111197763</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1396" s="3">
+        <v>1006688609</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1397" s="5">
+        <v>1121875236</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1398" s="3">
+        <v>1006778905</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1399" s="3">
+        <v>1122117276</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1400" s="5">
+        <v>1122138809</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1401" s="3">
+        <v>1123058148</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1402" s="3">
+        <v>1123565795</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1403" s="3">
+        <v>40341027</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1404" s="3">
+        <v>1120387069</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1405" s="3">
+        <v>1123564388</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1406" s="5">
+        <v>1123512956</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1407" s="5">
+        <v>1121416747</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1408" s="3">
+        <v>1020824438</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1409" s="3">
+        <v>1000834345</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1410" s="3">
+        <v>1193547301</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1411" s="3">
+        <v>20699563</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1412" s="5">
+        <v>1120498474</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1413" s="3">
+        <v>1006779481</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1414" s="3">
+        <v>41241858</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1415" s="5">
+        <v>1123114456</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1416" s="5">
+        <v>40405695</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1417" s="3">
+        <v>52096535</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1418" s="3">
+        <v>1120472391</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1419" s="5">
+        <v>1120372119</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1420" s="5">
+        <v>1123114061</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1421" s="5">
+        <v>1121903090</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1422" s="3">
+        <v>1123087731</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1423" s="3">
+        <v>1122144884</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1424" s="3">
+        <v>1015996912</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1425" s="3">
+        <v>1121905136</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1426" s="3">
+        <v>1120924575</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1427" s="3">
+        <v>1122125305</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1428" s="3">
+        <v>1006777428</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1429" s="3">
+        <v>1118020889</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1430" s="3">
+        <v>1122918095</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1431" s="3">
+        <v>1120352059</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1432" s="5">
+        <v>1116505062</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1433" s="3">
+        <v>1003530338</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1434" s="3">
+        <v>1121953048</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1435" s="3">
+        <v>1005856097</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1436" s="3">
+        <v>1123863140</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1437" s="5">
+        <v>1006697920</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1438" s="5">
+        <v>40265478</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1439" s="3">
+        <v>1023367834</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1440" s="3">
+        <v>1120844914</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1441" s="5">
+        <v>1123085348</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1442" s="3">
+        <v>1121872052</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1443" s="3">
+        <v>1006876003</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1444" s="3">
+        <v>1072593142</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1445" s="3">
+        <v>1006794764</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1446" s="3">
+        <v>1120924057</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1447" s="5">
+        <v>1120006623</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1448" s="3">
+        <v>1122626591</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1449" s="3">
+        <v>30946278</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1450" s="5">
+        <v>1122646404</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1451" s="3">
+        <v>80904798</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1452" s="3">
+        <v>1122132070</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1453" s="5">
+        <v>1056771673</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1454" s="5">
+        <v>21991161</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1455" s="5">
+        <v>40445242</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1456" s="5">
+        <v>1120381379</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1457" s="5">
+        <v>1121921932</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1458" s="3">
+        <v>1120818086</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1459" s="3">
+        <v>1122123029</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1460" s="5">
+        <v>1000693714</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1461" s="3">
+        <v>1096037708</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1462" s="3">
+        <v>1122143934</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1463" s="3">
+        <v>1006692935</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1464" s="5">
+        <v>1005319257</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1465" s="5">
+        <v>1193112708</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1466" s="3">
+        <v>1120560790</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1467" s="3">
+        <v>1122139765</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1468" s="3">
+        <v>1033740918</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1469" s="3">
+        <v>1090438876</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1470" s="3">
+        <v>1122119691</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1471" s="3">
+        <v>1123864028</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1472" s="5">
+        <v>1120355934</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1473" s="5">
+        <v>1016945097</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1474" s="3">
+        <v>1122653258</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1475" s="5">
+        <v>1006777121</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1476" s="3">
+        <v>65783261</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1477" s="5">
+        <v>1121146244</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1478" s="5">
+        <v>1123515171</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1479" s="3">
+        <v>1006866651</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1480" s="3">
+        <v>1001270374</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1481" s="3">
+        <v>1120504886</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1482" s="3">
+        <v>1234788097</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1483" s="5">
+        <v>1006874253</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1484" s="5">
+        <v>1123567290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parametrizacion de cedulas con cierre de sesion para ejecutar el dia: 10/08/2025 en la noche
</commit_message>
<xml_diff>
--- a/cedulas_Procesadas.xlsx
+++ b/cedulas_Procesadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ContratosSuperflex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9559C06F-C09E-41D2-AEC6-9B1A48AE0025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95059EA4-0D9A-4BD1-90B6-6DDB0398F690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1762"/>
+  <dimension ref="A1:F1905"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1671" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1688" sqref="B1688"/>
+    <sheetView tabSelected="1" topLeftCell="A1726" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1743" sqref="B1743"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9265,6 +9265,716 @@
         <v>1123567290</v>
       </c>
     </row>
+    <row r="1764" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1764" s="1">
+        <v>45938</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1765" s="5">
+        <v>21205258</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1766" s="3">
+        <v>31006459</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1767" s="5">
+        <v>11373533</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1768" s="5">
+        <v>30030456</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1769" s="5">
+        <v>70052315</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1770" s="3">
+        <v>40449322</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1771" s="3">
+        <v>40329872</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1772" s="3">
+        <v>40219846</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1773" s="3">
+        <v>1122338100</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1774" s="5">
+        <v>17303753</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1775" s="5">
+        <v>17345135</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1776" s="3">
+        <v>33875522</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1777" s="3">
+        <v>36293795</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1778" s="3">
+        <v>20871642</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1779" s="3">
+        <v>40186554</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1780" s="7">
+        <v>52287828</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1781" s="7">
+        <v>40333471</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1782" s="7">
+        <v>50976844</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1783" s="7">
+        <v>40329979</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1784" s="7">
+        <v>35263486</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1785" s="8">
+        <v>40415999</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1786" s="5">
+        <v>11405158</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1787" s="5">
+        <v>40384750</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1788" s="5">
+        <v>26508842</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1789" s="3">
+        <v>1121920935</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1790" s="3">
+        <v>30081591</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1791" s="3">
+        <v>40371629</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1792" s="3">
+        <v>1121840691</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1793" s="3">
+        <v>41213156</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1794" s="5">
+        <v>30080583</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1795" s="5">
+        <v>52812191</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1796" s="5">
+        <v>17329021</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1797" s="5">
+        <v>39728361</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1798" s="3">
+        <v>21011250</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1799" s="3">
+        <v>1120868086</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1800" s="3">
+        <v>21243208</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1801" s="3">
+        <v>1799801717</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1802" s="3">
+        <v>15960326</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1803" s="3">
+        <v>1120868173</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1804" s="3">
+        <v>900084777</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1805" s="3">
+        <v>1033690960</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1806" s="5">
+        <v>1075315269</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1807" s="3">
+        <v>33676007</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1808" s="3">
+        <v>1121818890</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1809" s="3">
+        <v>555555555</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1810" s="5">
+        <v>555555556</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1811" s="3">
+        <v>900737989</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1812" s="3">
+        <v>9007379890</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1813" s="3">
+        <v>1121913651</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1814" s="3">
+        <v>9000847773</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1815" s="3">
+        <v>9000847774</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1816" s="3">
+        <v>52861841</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1817" s="5">
+        <v>555555551</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1818" s="3">
+        <v>5849675</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1819" s="5">
+        <v>555555552</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1820" s="5">
+        <v>555555553</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1821" s="5">
+        <v>555555554</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1822" s="3">
+        <v>40417192</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1823" s="3">
+        <v>1122117543</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1824" s="3">
+        <v>1799831717</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1825" s="3">
+        <v>1799821717</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1826" s="3">
+        <v>1799841717</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1827" s="5">
+        <v>40416523</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1828" s="3">
+        <v>9000847771</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1829" s="3">
+        <v>9000847772</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1830" s="3">
+        <v>40188434</v>
+      </c>
+    </row>
+    <row r="1831" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1831" s="5">
+        <v>1121828917</v>
+      </c>
+    </row>
+    <row r="1832" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1832" s="3">
+        <v>1006771687</v>
+      </c>
+    </row>
+    <row r="1833" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1833" s="3">
+        <v>1118555784</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1834" s="3">
+        <v>79891869</v>
+      </c>
+    </row>
+    <row r="1835" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1835" s="3">
+        <v>40438899</v>
+      </c>
+    </row>
+    <row r="1836" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1836" s="3">
+        <v>555555557</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1837">
+        <v>68297670</v>
+      </c>
+    </row>
+    <row r="1838" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1838" s="5">
+        <v>14952515</v>
+      </c>
+    </row>
+    <row r="1839" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1839" s="3">
+        <v>1033723546</v>
+      </c>
+    </row>
+    <row r="1840" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1840" s="3">
+        <v>1120374995</v>
+      </c>
+    </row>
+    <row r="1841" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1841" s="3">
+        <v>86044711</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1842" s="3">
+        <v>40342629</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1843" s="3">
+        <v>1006720164</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1844" s="3">
+        <v>1121869388</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1845" s="5">
+        <v>890900608214</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1846" s="5">
+        <v>890900608211</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1847" s="3">
+        <v>555555558</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1848" s="5">
+        <v>89090060825</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1849" s="3">
+        <v>40356371</v>
+      </c>
+    </row>
+    <row r="1850" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1850" s="3">
+        <v>40218334</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1851" s="3">
+        <v>1108928812</v>
+      </c>
+    </row>
+    <row r="1852" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1852" s="3">
+        <v>9007505342</v>
+      </c>
+    </row>
+    <row r="1853" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1853" s="3">
+        <v>1003483201</v>
+      </c>
+    </row>
+    <row r="1854" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1854" s="3">
+        <v>1121911590</v>
+      </c>
+    </row>
+    <row r="1855" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1855" s="3">
+        <v>30080723</v>
+      </c>
+    </row>
+    <row r="1856" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1856" s="3">
+        <v>1006779023</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1857" s="5">
+        <v>8909006082</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1858" s="5">
+        <v>890900608213</v>
+      </c>
+    </row>
+    <row r="1859" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1859" s="5">
+        <v>89090060821</v>
+      </c>
+    </row>
+    <row r="1860" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1860" s="5">
+        <v>89090060829</v>
+      </c>
+    </row>
+    <row r="1861" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1861" s="5">
+        <v>890900608212</v>
+      </c>
+    </row>
+    <row r="1862" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1862" s="5">
+        <v>89090060824</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1863" s="5">
+        <v>89090060827</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1864" s="5">
+        <v>89090060828</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1865" s="5">
+        <v>890900608210</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1866" s="3">
+        <v>40305749</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1867" s="3">
+        <v>1006718970</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1868" s="3">
+        <v>1122919735</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1869" s="3">
+        <v>1006859801</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1870" s="3">
+        <v>1004634852</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1871" s="3">
+        <v>1116809197</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1872" s="3">
+        <v>444444444</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1873" s="3">
+        <v>40330136</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1874" s="3">
+        <v>1038100731</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1875" s="3">
+        <v>1116861125</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1876" s="3">
+        <v>1120866044</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1877" s="3">
+        <v>69022144</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1878" s="3">
+        <v>1121820427</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1879" s="3">
+        <v>1053764354</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1880" s="3">
+        <v>1011086251</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1881" s="3">
+        <v>1121849836</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1882" s="3">
+        <v>1120864873</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1883" s="3">
+        <v>1133839243</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1884" s="3">
+        <v>1121968001</v>
+      </c>
+    </row>
+    <row r="1885" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1885" s="3">
+        <v>77777778</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1886" s="3">
+        <v>77777779</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1887" s="3">
+        <v>1006719384</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1888" s="3">
+        <v>1006858033</v>
+      </c>
+    </row>
+    <row r="1889" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1889" s="5">
+        <v>1122922330</v>
+      </c>
+    </row>
+    <row r="1890" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1890" s="3">
+        <v>1082773285</v>
+      </c>
+    </row>
+    <row r="1891" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1891" s="3">
+        <v>55190862</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1892" s="3">
+        <v>1070325222</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1893" s="3">
+        <v>30520140</v>
+      </c>
+    </row>
+    <row r="1894" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1894" s="3">
+        <v>1124818008</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1895" s="3">
+        <v>444444441</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1896" s="3">
+        <v>444444442</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1897" s="3">
+        <v>444444443</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1898" s="3">
+        <v>1006719691</v>
+      </c>
+    </row>
+    <row r="1899" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1899" s="3">
+        <v>1121946622</v>
+      </c>
+    </row>
+    <row r="1900" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1900" s="3">
+        <v>1006720627</v>
+      </c>
+    </row>
+    <row r="1901" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1901" s="3">
+        <v>1123565052</v>
+      </c>
+    </row>
+    <row r="1902" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1902" s="3">
+        <v>40413517</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1903" s="3">
+        <v>63251940</v>
+      </c>
+    </row>
+    <row r="1904" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1904" s="3">
+        <v>1006009495</v>
+      </c>
+    </row>
+    <row r="1905" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1905" s="3">
+        <v>1002596538</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1090:B1128"/>

</xml_diff>